<commit_message>
update statistic and/or edit method
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\quan-ly-thuoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751130D4-50D2-4234-A49F-FCDF380B9FBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEE3A5D-8660-4108-8AB1-88878C969FB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,48 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>ThuocDemo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Ab</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Square</t>
-  </si>
-  <si>
-    <t>Io</t>
-  </si>
-  <si>
-    <t>ThuocDemo2</t>
-  </si>
-  <si>
-    <t>Blue</t>
+    <t>demoMed</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>Ma tuy</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
   <si>
     <t>Round</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>NOtTHuoc</t>
-  </si>
-  <si>
-    <t>NOT A COLOR</t>
-  </si>
-  <si>
-    <t>NOT A SHAPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,38 +367,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
       </c>
       <c r="D1">
         <v>1.5</v>
       </c>
       <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
         <v>100</v>
-      </c>
-      <c r="F1">
-        <v>120</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -418,9 +401,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -428,46 +411,20 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>1.2</v>
       </c>
-      <c r="E2">
-        <v>144</v>
-      </c>
-      <c r="F2">
-        <v>124</v>
+      <c r="E2" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>165.0</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>241</v>
-      </c>
-      <c r="E3">
-        <v>121</v>
-      </c>
-      <c r="F3">
-        <v>51616</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bo sung ham update
-Bay gio ham update co the xoa thuoc
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -418,50 +418,24 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>1.2</v>
+        <v>1.9</v>
       </c>
       <c r="E2" t="n">
-        <v>25.0</v>
+        <v>14.0</v>
       </c>
       <c r="F2" t="n">
-        <v>165.0</v>
+        <v>266.0</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E3" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>266.0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
don dep code+ them icon
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="12">
   <si>
     <t>Ab</t>
   </si>
@@ -404,7 +404,7 @@
         <v>10.0</v>
       </c>
       <c r="F1" t="n">
-        <v>114.0</v>
+        <v>282.0</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -456,7 +456,7 @@
         <v>14.0</v>
       </c>
       <c r="F3" t="n">
-        <v>266.0</v>
+        <v>1994.0</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
update import new medicine
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="22">
   <si>
     <t>Ab</t>
   </si>
@@ -61,6 +61,36 @@
   </si>
   <si>
     <t>Nein</t>
+  </si>
+  <si>
+    <t>Abxx</t>
+  </si>
+  <si>
+    <t>demoMednew</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>mai thuy</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>tron</t>
+  </si>
+  <si>
+    <t>hmm</t>
+  </si>
+  <si>
+    <t>thuoc te</t>
+  </si>
+  <si>
+    <t>tim</t>
+  </si>
+  <si>
+    <t>vuong</t>
   </si>
 </sst>
 </file>
@@ -379,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -387,30 +417,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="n">
         <v>1.0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D1" t="n">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="E1" t="n">
-        <v>10.0</v>
+        <v>14.0</v>
       </c>
       <c r="F1" t="n">
-        <v>282.0</v>
+        <v>2570.0</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -418,51 +448,77 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="E2" t="n">
-        <v>25.0</v>
+        <v>10.0</v>
       </c>
       <c r="F2" t="n">
-        <v>165.0</v>
+        <v>310.0</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
         <v>1.0</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.9</v>
-      </c>
       <c r="E3" t="n">
-        <v>14.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" t="n">
-        <v>1994.0</v>
+        <v>40.0</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>400.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update search menu+ don vi do
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\quan-ly-thuoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D986357F-3BF0-4868-9C5E-310343DA4CAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEE3A5D-8660-4108-8AB1-88878C969FB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Ab</t>
+  </si>
+  <si>
+    <t>demoMed</t>
+  </si>
   <si>
     <t>red</t>
   </si>
@@ -33,37 +39,25 @@
     <t>shape</t>
   </si>
   <si>
-    <t>MX-t11</t>
-  </si>
-  <si>
-    <t>Panadol</t>
-  </si>
-  <si>
-    <t>Yellowish</t>
-  </si>
-  <si>
-    <t>Nein</t>
-  </si>
-  <si>
-    <t>Abxx</t>
-  </si>
-  <si>
-    <t>demoMednew</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>rd</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>xjccx</t>
-  </si>
-  <si>
-    <t>aiojfc</t>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>Ma tuy</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Paracetamol</t>
+  </si>
+  <si>
+    <t>đỏ</t>
+  </si>
+  <si>
+    <t>hơi tròn</t>
   </si>
 </sst>
 </file>
@@ -382,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -395,76 +389,50 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1.5</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="D1">
-        <v>1.9</v>
-      </c>
-      <c r="E1">
-        <v>14</v>
-      </c>
-      <c r="F1">
-        <v>2570</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F2" t="n">
-        <v>11.0</v>
+        <v>225.0</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>